<commit_message>
Another day with CV
</commit_message>
<xml_diff>
--- a/data/Cross-validation/resumen.xlsx
+++ b/data/Cross-validation/resumen.xlsx
@@ -9,12 +9,13 @@
     <sheet name="lm" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="glm" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="randomForest" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="knn" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -25,7 +26,10 @@
     <t xml:space="preserve">bias</t>
   </si>
   <si>
-    <t xml:space="preserve">cor</t>
+    <t xml:space="preserve">cor1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cor2</t>
   </si>
   <si>
     <t xml:space="preserve">RMSE</t>
@@ -391,90 +395,108 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.249155611991692</v>
+        <v>0.356998431242402</v>
       </c>
       <c r="C2" t="n">
-        <v>0.999819249742929</v>
+        <v>1.00875263869728</v>
       </c>
       <c r="D2" t="n">
-        <v>0.460857862471004</v>
+        <v>0.552086240708944</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0755738988809654</v>
+        <v>0.426337282112785</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0844028528077384</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.366054876265934</v>
+        <v>0.39596828970968</v>
       </c>
       <c r="C3" t="n">
-        <v>1.00687921722579</v>
+        <v>1.01509176833617</v>
       </c>
       <c r="D3" t="n">
-        <v>0.547751342751</v>
+        <v>0.568361087528583</v>
       </c>
       <c r="E3" t="n">
-        <v>0.106598328223464</v>
+        <v>0.517560291044462</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.114226974056548</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.418521312456439</v>
+        <v>0.623553116802343</v>
       </c>
       <c r="C4" t="n">
-        <v>1.00675906426341</v>
+        <v>1.00774907911811</v>
       </c>
       <c r="D4" t="n">
-        <v>0.582803502196821</v>
+        <v>0.740450608175213</v>
       </c>
       <c r="E4" t="n">
-        <v>0.114670852870998</v>
+        <v>0.483941005009877</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.122890541132252</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.234433564480465</v>
+        <v>0.249214539534343</v>
       </c>
       <c r="C5" t="n">
-        <v>1.00222959902022</v>
+        <v>1.01142299048137</v>
       </c>
       <c r="D5" t="n">
-        <v>0.430882094455953</v>
+        <v>0.431418413758017</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0671393339560836</v>
+        <v>0.402512323377383</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0700250975727749</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.281406679919679</v>
+        <v>0.300304688464977</v>
       </c>
       <c r="C6" t="n">
-        <v>1.00072340354803</v>
+        <v>1.0049538872016</v>
       </c>
       <c r="D6" t="n">
-        <v>0.513346111481988</v>
+        <v>0.501817263513791</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0595799549900337</v>
+        <v>0.494460855914543</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0629765123633122</v>
       </c>
     </row>
   </sheetData>
@@ -507,90 +529,108 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.228789327191427</v>
+        <v>0.355682851764593</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0011845160825</v>
+        <v>0.999757505513779</v>
       </c>
       <c r="D2" t="n">
-        <v>0.444109423988044</v>
+        <v>0.566697826252613</v>
       </c>
       <c r="E2" t="n">
-        <v>29.7843478520252</v>
+        <v>0.429571041318111</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0831003921894197</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.378287990977889</v>
+        <v>0.397401740429509</v>
       </c>
       <c r="C3" t="n">
-        <v>1.01065580290917</v>
+        <v>1.00067369285668</v>
       </c>
       <c r="D3" t="n">
-        <v>0.528247473277434</v>
+        <v>0.574277788695762</v>
       </c>
       <c r="E3" t="n">
-        <v>41.9861468710106</v>
+        <v>0.51907014242039</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.113641500380643</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.254038948125374</v>
+        <v>0.628840182120175</v>
       </c>
       <c r="C4" t="n">
-        <v>0.997962137004635</v>
+        <v>1.00133507253272</v>
       </c>
       <c r="D4" t="n">
-        <v>0.476817500905577</v>
+        <v>0.728161871076884</v>
       </c>
       <c r="E4" t="n">
-        <v>46.7882484449894</v>
+        <v>0.482633404897965</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.125864862063917</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.292963629240173</v>
+        <v>0.249144669442368</v>
       </c>
       <c r="C5" t="n">
-        <v>1.00288129289753</v>
+        <v>1.00013433680816</v>
       </c>
       <c r="D5" t="n">
-        <v>0.506954935811483</v>
+        <v>0.434031265766093</v>
       </c>
       <c r="E5" t="n">
-        <v>27.96447280397</v>
+        <v>0.403684969393035</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0699160014350932</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.280214273080333</v>
+        <v>0.298298918013315</v>
       </c>
       <c r="C6" t="n">
-        <v>1.00132967241044</v>
+        <v>0.999724705744873</v>
       </c>
       <c r="D6" t="n">
-        <v>0.505161234703269</v>
+        <v>0.506789188959009</v>
       </c>
       <c r="E6" t="n">
-        <v>12.8547533347732</v>
+        <v>0.498322764429342</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0627125444755543</v>
       </c>
     </row>
   </sheetData>
@@ -623,90 +663,242 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.252612860706918</v>
+        <v>0.459824848727384</v>
       </c>
       <c r="C2" t="n">
-        <v>1.00360663166813</v>
+        <v>1.02436926363346</v>
       </c>
       <c r="D2" t="n">
-        <v>0.443548958496912</v>
+        <v>0.631902385956943</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0766528178664771</v>
+        <v>0.348674713822861</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.078140142844817</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.339153756401225</v>
+        <v>0.469121674351911</v>
       </c>
       <c r="C3" t="n">
-        <v>1.01144729282979</v>
+        <v>1.01517019750327</v>
       </c>
       <c r="D3" t="n">
-        <v>0.52441177599491</v>
+        <v>0.633623020824343</v>
       </c>
       <c r="E3" t="n">
-        <v>0.108823870401151</v>
+        <v>0.461580994381967</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.108656374507281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.386257640268027</v>
+        <v>0.630481516356916</v>
       </c>
       <c r="C4" t="n">
-        <v>1.00212807363687</v>
+        <v>1.00563755265042</v>
       </c>
       <c r="D4" t="n">
-        <v>0.582612151554416</v>
+        <v>0.764373174498036</v>
       </c>
       <c r="E4" t="n">
-        <v>0.114435499771541</v>
+        <v>0.409791018860439</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.114464054233356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.313593941516271</v>
+        <v>0.371148283548642</v>
       </c>
       <c r="C5" t="n">
-        <v>1.00604073251309</v>
+        <v>1.01727770806536</v>
       </c>
       <c r="D5" t="n">
-        <v>0.398295386268744</v>
+        <v>0.464223784349427</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0672782798786031</v>
+        <v>0.322631624997902</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0675322428447305</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.411292790334665</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.01031335079449</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.610790164026597</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.424258698899956</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0585189603330702</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.993061188896763</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.999069111035801</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.446463898863761</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.166378922887274</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.105559552304538</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.06714774953197</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.00339570979271</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.430246451282144</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.276068453452492</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.147158163469892</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.02401062559034</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.00783036493845</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.661847778321802</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.296779377150589</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.150204845491451</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="n">
+        <v>1.57816846432379</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.998758505285383</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.274939944402421</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.135988749341796</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0934634978501901</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" t="n">
-        <v>0.286090769794254</v>
+        <v>1.22979895225807</v>
       </c>
       <c r="C6" t="n">
-        <v>1.00673823723148</v>
+        <v>1.00754215929452</v>
       </c>
       <c r="D6" t="n">
-        <v>0.530521232675456</v>
+        <v>0.395971697514185</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0590509685279758</v>
+        <v>0.207192293035423</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0821613982076782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>